<commit_message>
Add readme and codes for final report
</commit_message>
<xml_diff>
--- a/src/main/resources/RADxStudyCodeList.xlsx
+++ b/src/main/resources/RADxStudyCodeList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\629441\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-metadata-evaluator/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{530FF0D2-77E2-4F35-8EDF-7A74FA237B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F67496C-1A19-6B48-8689-FBBD6ADFFA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="1" xr2:uid="{DB39AE42-C670-48C4-8F2A-F6A2F72DB77A}"/>
+    <workbookView xWindow="9120" yWindow="5500" windowWidth="29080" windowHeight="15760" activeTab="1" xr2:uid="{DB39AE42-C670-48C4-8F2A-F6A2F72DB77A}"/>
   </bookViews>
   <sheets>
     <sheet name="Code-Lists" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="217">
   <si>
     <t>Metadata Column</t>
   </si>
@@ -658,9 +658,6 @@
   </si>
   <si>
     <t>School Communities</t>
-  </si>
-  <si>
-    <t>DATA_TYPES</t>
   </si>
   <si>
     <t>Geospatial</t>
@@ -759,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -773,7 +770,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,10 +785,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1098,15 +1090,15 @@
       <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="58.5" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1142,7 +1134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1164,7 +1156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +1178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1197,7 +1189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1230,7 +1222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1241,7 +1233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1252,7 +1244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1263,7 +1255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1277,7 +1269,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1288,7 +1280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1299,7 +1291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1313,7 +1305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1327,7 +1319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1338,7 +1330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1349,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1360,7 +1352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -1374,7 +1366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -1399,7 +1391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1410,7 +1402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1421,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1432,7 +1424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1454,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1465,7 +1457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1487,7 +1479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1498,7 +1490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1509,7 +1501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1520,7 +1512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1531,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1542,7 +1534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1564,7 +1556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1575,7 +1567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -1586,7 +1578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1597,7 +1589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1608,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -1619,7 +1611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -1630,7 +1622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1641,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -1652,7 +1644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1663,7 +1655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1674,7 +1666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1685,7 +1677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1696,7 +1688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1707,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1718,7 +1710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1729,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1740,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -1751,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -1762,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -1773,7 +1765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -1784,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -1795,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -1806,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>54</v>
       </c>
@@ -1817,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -1828,7 +1820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -1839,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -1850,7 +1842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -1861,7 +1853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -1872,7 +1864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1883,7 +1875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -1894,7 +1886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -1905,7 +1897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -1916,7 +1908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -1927,7 +1919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -1938,7 +1930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1949,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1960,7 +1952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -1971,7 +1963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -1982,7 +1974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -1993,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -2004,7 +1996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -2015,7 +2007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -2026,7 +2018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -2037,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -2048,7 +2040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>74</v>
       </c>
@@ -2059,7 +2051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -2070,7 +2062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>74</v>
       </c>
@@ -2081,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>74</v>
       </c>
@@ -2092,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -2103,7 +2095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>74</v>
       </c>
@@ -2114,7 +2106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>74</v>
       </c>
@@ -2125,7 +2117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -2136,7 +2128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2147,7 +2139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -2158,7 +2150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -2169,7 +2161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -2180,7 +2172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>107</v>
       </c>
@@ -2191,7 +2183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -2202,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -2213,7 +2205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -2224,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -2235,7 +2227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -2246,7 +2238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -2257,7 +2249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -2268,7 +2260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -2279,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -2290,7 +2282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -2301,7 +2293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2312,7 +2304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2323,7 +2315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -2334,7 +2326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>107</v>
       </c>
@@ -2345,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -2356,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>107</v>
       </c>
@@ -2367,7 +2359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -2378,7 +2370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>107</v>
       </c>
@@ -2389,7 +2381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>107</v>
       </c>
@@ -2400,7 +2392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>107</v>
       </c>
@@ -2411,7 +2403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>107</v>
       </c>
@@ -2422,7 +2414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>107</v>
       </c>
@@ -2433,7 +2425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>107</v>
       </c>
@@ -2444,7 +2436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>107</v>
       </c>
@@ -2455,7 +2447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -2466,7 +2458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>107</v>
       </c>
@@ -2477,7 +2469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>107</v>
       </c>
@@ -2488,7 +2480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>107</v>
       </c>
@@ -2499,7 +2491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>107</v>
       </c>
@@ -2510,7 +2502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>107</v>
       </c>
@@ -2521,7 +2513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>107</v>
       </c>
@@ -2532,7 +2524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>107</v>
       </c>
@@ -2543,7 +2535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>107</v>
       </c>
@@ -2554,7 +2546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>107</v>
       </c>
@@ -2565,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>107</v>
       </c>
@@ -2576,7 +2568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -2587,7 +2579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>144</v>
       </c>
@@ -2598,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>144</v>
       </c>
@@ -2609,7 +2601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>144</v>
       </c>
@@ -2620,7 +2612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -2631,7 +2623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -2642,7 +2634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>144</v>
       </c>
@@ -2653,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>144</v>
       </c>
@@ -2664,7 +2656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>144</v>
       </c>
@@ -2675,7 +2667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>144</v>
       </c>
@@ -2686,7 +2678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>144</v>
       </c>
@@ -2697,7 +2689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -2708,7 +2700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -2719,7 +2711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -2730,7 +2722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>144</v>
       </c>
@@ -2741,7 +2733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>144</v>
       </c>
@@ -2752,7 +2744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>144</v>
       </c>
@@ -2763,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>144</v>
       </c>
@@ -2774,7 +2766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>144</v>
       </c>
@@ -2785,7 +2777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>144</v>
       </c>
@@ -2796,7 +2788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>144</v>
       </c>
@@ -2807,7 +2799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>144</v>
       </c>
@@ -2829,20 +2821,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A24D681-E7DF-41F3-ADBC-77AEEF509C99}">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="50.5" customWidth="1"/>
+    <col min="3" max="3" width="59.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2859,7 +2851,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2873,7 +2865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2887,7 +2879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2901,7 +2893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2915,7 +2907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2929,7 +2921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2943,7 +2935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2957,7 +2949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2971,7 +2963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2985,7 +2977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2999,7 +2991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -3014,7 +3006,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -3029,7 +3021,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -3043,7 +3035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3057,7 +3049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3071,7 +3063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -3085,7 +3077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3099,7 +3091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -3113,7 +3105,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3127,7 +3119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3141,7 +3133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -3155,7 +3147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3169,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -3183,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3197,7 +3189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3211,7 +3203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3225,7 +3217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3239,7 +3231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -3253,7 +3245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -3267,7 +3259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3281,72 +3273,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>205</v>
+    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>205</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -3360,7 +3352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3374,7 +3366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -3388,7 +3380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3402,7 +3394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -3416,7 +3408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3430,7 +3422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
@@ -3444,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>54</v>
       </c>
@@ -3458,7 +3450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
@@ -3472,7 +3464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -3486,7 +3478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -3500,7 +3492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -3514,7 +3506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -3528,7 +3520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -3542,7 +3534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -3556,7 +3548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3570,7 +3562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>71</v>
       </c>
@@ -3585,7 +3577,7 @@
       </c>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>71</v>
       </c>
@@ -3600,7 +3592,7 @@
       </c>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -3614,7 +3606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3628,7 +3620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -3642,7 +3634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -3656,7 +3648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3670,7 +3662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -3684,7 +3676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -3698,7 +3690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -3712,7 +3704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -3726,7 +3718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -3740,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -3754,7 +3746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -3768,7 +3760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -3782,7 +3774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -3796,7 +3788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3810,7 +3802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -3824,7 +3816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -3838,7 +3830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -3852,7 +3844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -3866,7 +3858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -3880,7 +3872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -3894,7 +3886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -3908,7 +3900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -3922,7 +3914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -3936,7 +3928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -3950,7 +3942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -3964,7 +3956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -3978,7 +3970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>101</v>
       </c>
@@ -3992,7 +3984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -4006,7 +3998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>101</v>
       </c>
@@ -4020,7 +4012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>101</v>
       </c>
@@ -4034,7 +4026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>107</v>
       </c>
@@ -4049,7 +4041,7 @@
       </c>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>107</v>
       </c>
@@ -4057,27 +4049,27 @@
         <v>109</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="7" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" t="s">
         <v>110</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" t="s">
         <v>110</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -4091,7 +4083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -4105,7 +4097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -4119,7 +4111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -4133,7 +4125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -4147,7 +4139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>107</v>
       </c>
@@ -4161,7 +4153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -4175,7 +4167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -4189,7 +4181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -4203,7 +4195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -4217,7 +4209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -4231,7 +4223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>107</v>
       </c>
@@ -4245,7 +4237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -4259,7 +4251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -4273,7 +4265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -4287,7 +4279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -4301,7 +4293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -4315,7 +4307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -4329,7 +4321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>107</v>
       </c>
@@ -4344,7 +4336,7 @@
       </c>
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>107</v>
       </c>
@@ -4359,7 +4351,7 @@
       </c>
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -4373,7 +4365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>107</v>
       </c>
@@ -4387,7 +4379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -4401,7 +4393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>107</v>
       </c>
@@ -4416,7 +4408,7 @@
       </c>
       <c r="E115" s="5"/>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>107</v>
       </c>
@@ -4430,7 +4422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>107</v>
       </c>
@@ -4444,7 +4436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>107</v>
       </c>
@@ -4458,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>107</v>
       </c>
@@ -4472,7 +4464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>107</v>
       </c>
@@ -4486,7 +4478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>107</v>
       </c>
@@ -4500,7 +4492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -4514,7 +4506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>107</v>
       </c>
@@ -4528,7 +4520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>107</v>
       </c>
@@ -4542,7 +4534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>144</v>
       </c>
@@ -4556,7 +4548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>144</v>
       </c>
@@ -4570,7 +4562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>144</v>
       </c>
@@ -4584,7 +4576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>144</v>
       </c>
@@ -4598,7 +4590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>144</v>
       </c>
@@ -4606,13 +4598,13 @@
         <v>149</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>144</v>
       </c>
@@ -4626,21 +4618,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="7" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>144</v>
       </c>
-      <c r="B131" s="7" t="s">
+      <c r="B131" t="s">
         <v>151</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" t="s">
         <v>151</v>
       </c>
-      <c r="D131" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>144</v>
       </c>
@@ -4655,7 +4647,7 @@
       </c>
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -4669,7 +4661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>144</v>
       </c>
@@ -4683,7 +4675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>144</v>
       </c>
@@ -4697,7 +4689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>144</v>
       </c>
@@ -4705,13 +4697,13 @@
         <v>156</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>144</v>
       </c>
@@ -4719,13 +4711,13 @@
         <v>157</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>144</v>
       </c>
@@ -4740,21 +4732,21 @@
       </c>
       <c r="E138" s="5"/>
     </row>
-    <row r="139" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="7" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>144</v>
       </c>
-      <c r="B139" s="7" t="s">
+      <c r="B139" t="s">
         <v>159</v>
       </c>
-      <c r="C139" s="7" t="s">
+      <c r="C139" t="s">
         <v>159</v>
       </c>
-      <c r="D139" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>144</v>
       </c>
@@ -4768,7 +4760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>144</v>
       </c>
@@ -4782,7 +4774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>144</v>
       </c>
@@ -4796,7 +4788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>144</v>
       </c>
@@ -4811,7 +4803,7 @@
       </c>
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -4825,7 +4817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -4839,7 +4831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -4860,6 +4852,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EAAD467C93B6324EB7AE2601D1877CC8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5522e64b66a74c87a09b286faa0556d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2" xmlns:ns4="2bea61d9-cae5-4d7b-9970-651d1d561367" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b66153946105f69d7f94f28570fe83b" ns3:_="" ns4:_="">
     <xsd:import namespace="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2"/>
@@ -5092,24 +5101,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4FFC42-2874-49F8-B537-27A4FB5C1B51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2bea61d9-cae5-4d7b-9970-651d1d561367"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6774199-D315-442D-90EE-321D388C8F7F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96B8FE34-B541-4598-963F-51F3A1C0BD6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5128,31 +5145,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6774199-D315-442D-90EE-321D388C8F7F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F4FFC42-2874-49F8-B537-27A4FB5C1B51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2bea61d9-cae5-4d7b-9970-651d1d561367"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1f2c1cb9-fb97-4c9c-b5d7-3cdef7345fe2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{51d9dc18-15ea-424b-b24d-55ab4d4e7519}" enabled="1" method="Privileged" siteId="{d5fe813e-0caa-432a-b2ac-d555aa91bd1c}" removed="0"/>

</xml_diff>